<commit_message>
changes 4th aug 2016
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Assignments" sheetId="1" r:id="rId1"/>
+    <sheet name="StudentDetails" sheetId="2" r:id="rId2"/>
+    <sheet name="RegistrationURL" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Assignment Type</t>
   </si>
@@ -115,13 +115,46 @@
   </si>
   <si>
     <t>QB Assignment</t>
+  </si>
+  <si>
+    <t>StudentId</t>
+  </si>
+  <si>
+    <t>StudentPwd</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>registrationURL</t>
+  </si>
+  <si>
+    <t>Aa123456</t>
+  </si>
+  <si>
+    <t>STUDENT 1</t>
+  </si>
+  <si>
+    <t>http://connectqastg.mheducation.com/class/k-ins-chemistry-section1</t>
+  </si>
+  <si>
+    <t>http://connectqastg.mheducation.com/class/-_-_123--fname--section-1-2</t>
+  </si>
+  <si>
+    <t>stgauguststudent1@gmail.com</t>
+  </si>
+  <si>
+    <t>STG AUGUST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +166,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -155,14 +196,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -464,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,24 +651,85 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="68" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>